<commit_message>
v1.36 boot switch ok
</commit_message>
<xml_diff>
--- a/hotter/docs/协议.xlsx
+++ b/hotter/docs/协议.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9060" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9060" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="102">
   <si>
     <t>4-20ma</t>
   </si>
@@ -817,6 +817,9 @@
     <t>1、第一次get请求版本号，返回值：{V1.0.0，seq数量，连接地址}，
 例如{v1.0.0,33,31.106.169.131/firmware/}
 2、接下来控制板主动get请求读固件数据，返回值：1024个有效数据(不满1024为最后实际数据)+2crc</t>
+  </si>
+  <si>
+    <t>固件以现场名一样，中间有空格，例如现场A V1.0</t>
   </si>
   <si>
     <t>A</t>
@@ -2123,8 +2126,8 @@
   <sheetPr/>
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="7"/>
@@ -2521,8 +2524,8 @@
   <sheetPr/>
   <dimension ref="D7:I49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -2610,7 +2613,9 @@
       </c>
     </row>
     <row r="47" spans="4:4">
-      <c r="D47" s="4"/>
+      <c r="D47" s="4" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="48" spans="4:4">
       <c r="D48" s="4"/>
@@ -2638,33 +2643,33 @@
   <sheetData>
     <row r="1" spans="2:9">
       <c r="B1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>